<commit_message>
update ancillary files to be consistent with new yaml files
</commit_message>
<xml_diff>
--- a/Documentation/ArchetypeOffshoreSites-DistributionParameters.xlsx
+++ b/Documentation/ArchetypeOffshoreSites-DistributionParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E682BE9A-0355-D34C-8ADA-F73AC3D4DFE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A43186-0778-914E-A6A8-DAAB534D4045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="16320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attribution" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1051,38 +1054,31 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1114,8 +1110,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1129,29 +1155,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1493,7 +1496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1532,7 +1535,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="90" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1550,7 +1553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945F79CD-77E2-E04A-9001-62E98A2D50D8}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1573,44 +1576,44 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="E5" s="116" t="s">
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="E5" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="115"/>
-      <c r="G5" s="117" t="s">
+      <c r="F5" s="89"/>
+      <c r="G5" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="117"/>
-      <c r="I5" s="117"/>
-      <c r="J5" s="117"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="93"/>
     </row>
     <row r="6" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="114" t="s">
+      <c r="A6" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="114" t="s">
+      <c r="B6" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="114" t="s">
+      <c r="C6" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="116"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="114" t="s">
+      <c r="E6" s="92"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="114" t="s">
+      <c r="H6" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="114" t="s">
+      <c r="I6" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="114" t="s">
+      <c r="J6" s="88" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1624,14 +1627,14 @@
       <c r="C7" s="77">
         <v>8.5153824354742298</v>
       </c>
-      <c r="E7" s="112">
+      <c r="E7" s="86">
         <v>-1811332072</v>
       </c>
-      <c r="F7" s="111"/>
+      <c r="F7" s="85"/>
       <c r="G7" s="77">
         <v>1</v>
       </c>
-      <c r="H7" s="113">
+      <c r="H7" s="87">
         <v>40</v>
       </c>
       <c r="I7" s="77">
@@ -1651,10 +1654,10 @@
       <c r="C8" s="77">
         <v>8.3100636877459593</v>
       </c>
-      <c r="E8" s="112">
+      <c r="E8" s="86">
         <v>13173288</v>
       </c>
-      <c r="F8" s="111"/>
+      <c r="F8" s="85"/>
       <c r="G8" s="77">
         <v>50</v>
       </c>
@@ -1678,13 +1681,13 @@
       <c r="C9" s="77">
         <v>8.0063008892254803</v>
       </c>
-      <c r="E9" s="112">
+      <c r="E9" s="86">
         <v>-1472715972</v>
       </c>
-      <c r="F9" s="111"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
+      <c r="F9" s="85"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="77">
@@ -1696,13 +1699,13 @@
       <c r="C10" s="77">
         <v>7.6514231001636599</v>
       </c>
-      <c r="E10" s="112">
+      <c r="E10" s="86">
         <v>2098744693</v>
       </c>
-      <c r="F10" s="111"/>
-      <c r="H10" s="110"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="110"/>
+      <c r="F10" s="85"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="84"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="77">
@@ -1714,13 +1717,13 @@
       <c r="C11" s="77">
         <v>7.4405813379261296</v>
       </c>
-      <c r="E11" s="112">
+      <c r="E11" s="86">
         <v>185130004</v>
       </c>
-      <c r="F11" s="111"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="110"/>
+      <c r="F11" s="85"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="84"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="77">
@@ -1732,13 +1735,13 @@
       <c r="C12" s="77">
         <v>7.46083406332734</v>
       </c>
-      <c r="E12" s="112">
+      <c r="E12" s="86">
         <v>-802506215</v>
       </c>
-      <c r="F12" s="111"/>
-      <c r="H12" s="110"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="110"/>
+      <c r="F12" s="85"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="77">
@@ -1750,9 +1753,9 @@
       <c r="C13" s="77">
         <v>7.6433003065214402</v>
       </c>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="84"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="77">
@@ -1764,9 +1767,9 @@
       <c r="C14" s="77">
         <v>8.0468999417592002</v>
       </c>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="84"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="77">
@@ -1778,9 +1781,9 @@
       <c r="C15" s="77">
         <v>8.5213141052297097</v>
       </c>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="110"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="77">
@@ -1792,9 +1795,9 @@
       <c r="C16" s="77">
         <v>8.9870210237036208</v>
       </c>
-      <c r="H16" s="110"/>
-      <c r="I16" s="110"/>
-      <c r="J16" s="110"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="77">
@@ -1895,18 +1898,18 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="98" t="s">
+      <c r="G5" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="100"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="99"/>
     </row>
     <row r="6" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
@@ -1928,21 +1931,21 @@
       <c r="G6" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="90" t="s">
+      <c r="H6" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
       <c r="K6" s="105" t="s">
         <v>20</v>
       </c>
       <c r="L6" s="105"/>
       <c r="M6" s="105"/>
-      <c r="N6" s="101" t="s">
+      <c r="N6" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="101"/>
-      <c r="P6" s="102"/>
+      <c r="O6" s="100"/>
+      <c r="P6" s="101"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
@@ -1960,22 +1963,22 @@
       <c r="G7" s="66">
         <v>4</v>
       </c>
-      <c r="H7" s="91">
+      <c r="H7" s="106">
         <v>1.10191703260514</v>
       </c>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91">
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106">
         <v>8.5153824354742298</v>
       </c>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="103">
+      <c r="L7" s="106"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="102">
         <f>D7*180/PI()</f>
         <v>-20.81915116155221</v>
       </c>
-      <c r="O7" s="103"/>
-      <c r="P7" s="104"/>
+      <c r="O7" s="102"/>
+      <c r="P7" s="103"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
@@ -1993,22 +1996,22 @@
       <c r="G8" s="64">
         <v>6</v>
       </c>
-      <c r="H8" s="92">
+      <c r="H8" s="107">
         <v>1.1790526485225601</v>
       </c>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92">
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="107">
         <v>8.3100636877459593</v>
       </c>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92"/>
-      <c r="N8" s="94">
+      <c r="L8" s="107"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="91">
         <f>D8*180/PI()</f>
         <v>-28.554002304083379</v>
       </c>
-      <c r="O8" s="94"/>
-      <c r="P8" s="95"/>
+      <c r="O8" s="91"/>
+      <c r="P8" s="94"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
@@ -2026,22 +2029,22 @@
       <c r="G9" s="64">
         <v>8</v>
       </c>
-      <c r="H9" s="92">
+      <c r="H9" s="107">
         <v>1.3157151535593601</v>
       </c>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92">
+      <c r="I9" s="107"/>
+      <c r="J9" s="107"/>
+      <c r="K9" s="107">
         <v>8.0063008892254803</v>
       </c>
-      <c r="L9" s="92"/>
-      <c r="M9" s="92"/>
-      <c r="N9" s="94">
+      <c r="L9" s="107"/>
+      <c r="M9" s="107"/>
+      <c r="N9" s="91">
         <f t="shared" ref="N9:N17" si="0">D9*180/PI()</f>
         <v>-27.38277537649731</v>
       </c>
-      <c r="O9" s="94"/>
-      <c r="P9" s="95"/>
+      <c r="O9" s="91"/>
+      <c r="P9" s="94"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
@@ -2059,22 +2062,22 @@
       <c r="G10" s="64">
         <v>10</v>
       </c>
-      <c r="H10" s="92">
+      <c r="H10" s="107">
         <v>1.5368671240461</v>
       </c>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92">
+      <c r="I10" s="107"/>
+      <c r="J10" s="107"/>
+      <c r="K10" s="107">
         <v>7.6514231001636599</v>
       </c>
-      <c r="L10" s="92"/>
-      <c r="M10" s="92"/>
-      <c r="N10" s="94">
+      <c r="L10" s="107"/>
+      <c r="M10" s="107"/>
+      <c r="N10" s="91">
         <f t="shared" si="0"/>
         <v>-19.403504846181495</v>
       </c>
-      <c r="O10" s="94"/>
-      <c r="P10" s="95"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="94"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
@@ -2092,22 +2095,22 @@
       <c r="G11" s="64">
         <v>12</v>
       </c>
-      <c r="H11" s="92">
+      <c r="H11" s="107">
         <v>1.8358165142215901</v>
       </c>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92">
+      <c r="I11" s="107"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="107">
         <v>7.4405813379261296</v>
       </c>
-      <c r="L11" s="92"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="94">
+      <c r="L11" s="107"/>
+      <c r="M11" s="107"/>
+      <c r="N11" s="91">
         <f t="shared" si="0"/>
         <v>-12.289921542768647</v>
       </c>
-      <c r="O11" s="94"/>
-      <c r="P11" s="95"/>
+      <c r="O11" s="91"/>
+      <c r="P11" s="94"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
@@ -2125,22 +2128,22 @@
       <c r="G12" s="64">
         <v>14</v>
       </c>
-      <c r="H12" s="92">
+      <c r="H12" s="107">
         <v>2.1879946383206001</v>
       </c>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92">
+      <c r="I12" s="107"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="107">
         <v>7.46083406332734</v>
       </c>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92"/>
-      <c r="N12" s="94">
+      <c r="L12" s="107"/>
+      <c r="M12" s="107"/>
+      <c r="N12" s="91">
         <f t="shared" si="0"/>
         <v>-10.393865575279683</v>
       </c>
-      <c r="O12" s="94"/>
-      <c r="P12" s="95"/>
+      <c r="O12" s="91"/>
+      <c r="P12" s="94"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
@@ -2158,22 +2161,22 @@
       <c r="G13" s="64">
         <v>16</v>
       </c>
-      <c r="H13" s="92">
+      <c r="H13" s="107">
         <v>2.5981270962871599</v>
       </c>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="92">
+      <c r="I13" s="107"/>
+      <c r="J13" s="107"/>
+      <c r="K13" s="107">
         <v>7.6433003065214402</v>
       </c>
-      <c r="L13" s="92"/>
-      <c r="M13" s="92"/>
-      <c r="N13" s="94">
+      <c r="L13" s="107"/>
+      <c r="M13" s="107"/>
+      <c r="N13" s="91">
         <f t="shared" si="0"/>
         <v>-7.1538223649121919</v>
       </c>
-      <c r="O13" s="94"/>
-      <c r="P13" s="95"/>
+      <c r="O13" s="91"/>
+      <c r="P13" s="94"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
@@ -2191,22 +2194,22 @@
       <c r="G14" s="64">
         <v>18</v>
       </c>
-      <c r="H14" s="92">
+      <c r="H14" s="107">
         <v>3.0613040681969101</v>
       </c>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92">
+      <c r="I14" s="107"/>
+      <c r="J14" s="107"/>
+      <c r="K14" s="107">
         <v>8.0468999417592002</v>
       </c>
-      <c r="L14" s="92"/>
-      <c r="M14" s="92"/>
-      <c r="N14" s="94">
+      <c r="L14" s="107"/>
+      <c r="M14" s="107"/>
+      <c r="N14" s="91">
         <f t="shared" si="0"/>
         <v>-4.8135086428030176</v>
       </c>
-      <c r="O14" s="94"/>
-      <c r="P14" s="95"/>
+      <c r="O14" s="91"/>
+      <c r="P14" s="94"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
@@ -2224,22 +2227,22 @@
       <c r="G15" s="64">
         <v>20</v>
       </c>
-      <c r="H15" s="92">
+      <c r="H15" s="107">
         <v>3.6170354427381901</v>
       </c>
-      <c r="I15" s="92"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="92">
+      <c r="I15" s="107"/>
+      <c r="J15" s="107"/>
+      <c r="K15" s="107">
         <v>8.5213141052297097</v>
       </c>
-      <c r="L15" s="92"/>
-      <c r="M15" s="92"/>
-      <c r="N15" s="94">
+      <c r="L15" s="107"/>
+      <c r="M15" s="107"/>
+      <c r="N15" s="91">
         <f t="shared" si="0"/>
         <v>-1.5489446055955596</v>
       </c>
-      <c r="O15" s="94"/>
-      <c r="P15" s="95"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="94"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
@@ -2257,22 +2260,22 @@
       <c r="G16" s="64">
         <v>22</v>
       </c>
-      <c r="H16" s="92">
+      <c r="H16" s="107">
         <v>4.0274702192574798</v>
       </c>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92">
+      <c r="I16" s="107"/>
+      <c r="J16" s="107"/>
+      <c r="K16" s="107">
         <v>8.9870210237036208</v>
       </c>
-      <c r="L16" s="92"/>
-      <c r="M16" s="92"/>
-      <c r="N16" s="94">
+      <c r="L16" s="107"/>
+      <c r="M16" s="107"/>
+      <c r="N16" s="91">
         <f t="shared" si="0"/>
         <v>5.4345837534091519</v>
       </c>
-      <c r="O16" s="94"/>
-      <c r="P16" s="95"/>
+      <c r="O16" s="91"/>
+      <c r="P16" s="94"/>
     </row>
     <row r="17" spans="1:54" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
@@ -2290,22 +2293,22 @@
       <c r="G17" s="65">
         <v>24</v>
       </c>
-      <c r="H17" s="93">
+      <c r="H17" s="104">
         <v>4.5158067101122104</v>
       </c>
-      <c r="I17" s="93"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93">
+      <c r="I17" s="104"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="104">
         <v>9.4516410255313801</v>
       </c>
-      <c r="L17" s="93"/>
-      <c r="M17" s="93"/>
-      <c r="N17" s="96">
+      <c r="L17" s="104"/>
+      <c r="M17" s="104"/>
+      <c r="N17" s="95">
         <f t="shared" si="0"/>
         <v>7.0446550053850512</v>
       </c>
-      <c r="O17" s="96"/>
-      <c r="P17" s="97"/>
+      <c r="O17" s="95"/>
+      <c r="P17" s="96"/>
     </row>
     <row r="18" spans="1:54" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -2320,60 +2323,60 @@
       <c r="B19" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85"/>
-      <c r="P19" s="85"/>
-      <c r="Q19" s="85"/>
-      <c r="R19" s="85"/>
-      <c r="S19" s="85"/>
-      <c r="T19" s="85"/>
-      <c r="U19" s="85"/>
-      <c r="V19" s="85"/>
-      <c r="W19" s="85"/>
-      <c r="X19" s="85"/>
-      <c r="Y19" s="85"/>
-      <c r="Z19" s="85"/>
-      <c r="AA19" s="86"/>
-      <c r="AD19" s="84" t="s">
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
+      <c r="G19" s="109"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="109"/>
+      <c r="K19" s="109"/>
+      <c r="L19" s="109"/>
+      <c r="M19" s="109"/>
+      <c r="N19" s="109"/>
+      <c r="O19" s="109"/>
+      <c r="P19" s="109"/>
+      <c r="Q19" s="109"/>
+      <c r="R19" s="109"/>
+      <c r="S19" s="109"/>
+      <c r="T19" s="109"/>
+      <c r="U19" s="109"/>
+      <c r="V19" s="109"/>
+      <c r="W19" s="109"/>
+      <c r="X19" s="109"/>
+      <c r="Y19" s="109"/>
+      <c r="Z19" s="109"/>
+      <c r="AA19" s="110"/>
+      <c r="AD19" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="AE19" s="85"/>
-      <c r="AF19" s="85"/>
-      <c r="AG19" s="85"/>
-      <c r="AH19" s="85"/>
-      <c r="AI19" s="85"/>
-      <c r="AJ19" s="85"/>
-      <c r="AK19" s="85"/>
-      <c r="AL19" s="85"/>
-      <c r="AM19" s="85"/>
-      <c r="AN19" s="85"/>
-      <c r="AO19" s="85"/>
-      <c r="AP19" s="85"/>
-      <c r="AQ19" s="85"/>
-      <c r="AR19" s="85"/>
-      <c r="AS19" s="85"/>
-      <c r="AT19" s="85"/>
-      <c r="AU19" s="85"/>
-      <c r="AV19" s="85"/>
-      <c r="AW19" s="85"/>
-      <c r="AX19" s="85"/>
-      <c r="AY19" s="85"/>
-      <c r="AZ19" s="85"/>
-      <c r="BA19" s="85"/>
-      <c r="BB19" s="86"/>
+      <c r="AE19" s="109"/>
+      <c r="AF19" s="109"/>
+      <c r="AG19" s="109"/>
+      <c r="AH19" s="109"/>
+      <c r="AI19" s="109"/>
+      <c r="AJ19" s="109"/>
+      <c r="AK19" s="109"/>
+      <c r="AL19" s="109"/>
+      <c r="AM19" s="109"/>
+      <c r="AN19" s="109"/>
+      <c r="AO19" s="109"/>
+      <c r="AP19" s="109"/>
+      <c r="AQ19" s="109"/>
+      <c r="AR19" s="109"/>
+      <c r="AS19" s="109"/>
+      <c r="AT19" s="109"/>
+      <c r="AU19" s="109"/>
+      <c r="AV19" s="109"/>
+      <c r="AW19" s="109"/>
+      <c r="AX19" s="109"/>
+      <c r="AY19" s="109"/>
+      <c r="AZ19" s="109"/>
+      <c r="BA19" s="109"/>
+      <c r="BB19" s="110"/>
     </row>
     <row r="20" spans="1:54" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -4277,45 +4280,45 @@
       <c r="B34" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
-      <c r="H34" s="88"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="88"/>
-      <c r="K34" s="88"/>
-      <c r="L34" s="88"/>
-      <c r="M34" s="88"/>
-      <c r="N34" s="88"/>
-      <c r="O34" s="88"/>
-      <c r="P34" s="88"/>
-      <c r="Q34" s="88"/>
-      <c r="R34" s="88"/>
-      <c r="S34" s="89"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="112"/>
+      <c r="H34" s="112"/>
+      <c r="I34" s="112"/>
+      <c r="J34" s="112"/>
+      <c r="K34" s="112"/>
+      <c r="L34" s="112"/>
+      <c r="M34" s="112"/>
+      <c r="N34" s="112"/>
+      <c r="O34" s="112"/>
+      <c r="P34" s="112"/>
+      <c r="Q34" s="112"/>
+      <c r="R34" s="112"/>
+      <c r="S34" s="113"/>
       <c r="T34" s="20"/>
-      <c r="U34" s="87" t="s">
+      <c r="U34" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="V34" s="88"/>
-      <c r="W34" s="88"/>
-      <c r="X34" s="88"/>
-      <c r="Y34" s="88"/>
-      <c r="Z34" s="88"/>
-      <c r="AA34" s="88"/>
-      <c r="AB34" s="88"/>
-      <c r="AC34" s="88"/>
-      <c r="AD34" s="88"/>
-      <c r="AE34" s="88"/>
-      <c r="AF34" s="88"/>
-      <c r="AG34" s="88"/>
-      <c r="AH34" s="88"/>
-      <c r="AI34" s="88"/>
-      <c r="AJ34" s="88"/>
-      <c r="AK34" s="89"/>
+      <c r="V34" s="112"/>
+      <c r="W34" s="112"/>
+      <c r="X34" s="112"/>
+      <c r="Y34" s="112"/>
+      <c r="Z34" s="112"/>
+      <c r="AA34" s="112"/>
+      <c r="AB34" s="112"/>
+      <c r="AC34" s="112"/>
+      <c r="AD34" s="112"/>
+      <c r="AE34" s="112"/>
+      <c r="AF34" s="112"/>
+      <c r="AG34" s="112"/>
+      <c r="AH34" s="112"/>
+      <c r="AI34" s="112"/>
+      <c r="AJ34" s="112"/>
+      <c r="AK34" s="113"/>
     </row>
     <row r="35" spans="1:37" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
@@ -5633,6 +5636,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="C19:AA19"/>
+    <mergeCell ref="AD19:BB19"/>
+    <mergeCell ref="C34:S34"/>
+    <mergeCell ref="U34:AK34"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
     <mergeCell ref="N16:P16"/>
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="G5:P5"/>
@@ -5649,31 +5677,6 @@
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="C19:AA19"/>
-    <mergeCell ref="AD19:BB19"/>
-    <mergeCell ref="C34:S34"/>
-    <mergeCell ref="U34:AK34"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K13:M13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5759,18 +5762,18 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="98" t="s">
+      <c r="G5" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="100"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="99"/>
     </row>
     <row r="6" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
@@ -5792,21 +5795,21 @@
       <c r="G6" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="109" t="s">
+      <c r="H6" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="101" t="s">
+      <c r="I6" s="118"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101" t="s">
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="101"/>
-      <c r="P6" s="102"/>
+      <c r="O6" s="100"/>
+      <c r="P6" s="101"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
@@ -5824,22 +5827,22 @@
       <c r="G7" s="66">
         <v>4</v>
       </c>
-      <c r="H7" s="103">
+      <c r="H7" s="102">
         <v>1.9085675679482501</v>
       </c>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="103">
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="102">
         <v>12.2364570101645</v>
       </c>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
-      <c r="N7" s="103">
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102">
         <f>D7*180/PI()</f>
         <v>-23.797795230628868</v>
       </c>
-      <c r="O7" s="103"/>
-      <c r="P7" s="104"/>
+      <c r="O7" s="102"/>
+      <c r="P7" s="103"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
@@ -5857,22 +5860,22 @@
       <c r="G8" s="64">
         <v>6</v>
       </c>
-      <c r="H8" s="94">
+      <c r="H8" s="91">
         <v>1.96016259488156</v>
       </c>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94">
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91">
         <v>12.144977773946501</v>
       </c>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="94">
+      <c r="L8" s="91"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91">
         <f t="shared" ref="N8:N17" si="0">D8*180/PI()</f>
         <v>-23.792824531798669</v>
       </c>
-      <c r="O8" s="94"/>
-      <c r="P8" s="95"/>
+      <c r="O8" s="91"/>
+      <c r="P8" s="94"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
@@ -5890,22 +5893,22 @@
       <c r="G9" s="64">
         <v>8</v>
       </c>
-      <c r="H9" s="94">
+      <c r="H9" s="91">
         <v>2.0627222435468902</v>
       </c>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94">
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91">
         <v>11.9025494686445</v>
       </c>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="94">
+      <c r="L9" s="91"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="91">
         <f t="shared" si="0"/>
         <v>-22.390686750853625</v>
       </c>
-      <c r="O9" s="94"/>
-      <c r="P9" s="95"/>
+      <c r="O9" s="91"/>
+      <c r="P9" s="94"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
@@ -5923,22 +5926,22 @@
       <c r="G10" s="64">
         <v>10</v>
       </c>
-      <c r="H10" s="94">
+      <c r="H10" s="91">
         <v>2.2245394147192799</v>
       </c>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94">
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91">
         <v>11.519666597043701</v>
       </c>
-      <c r="L10" s="94"/>
-      <c r="M10" s="94"/>
-      <c r="N10" s="94">
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91">
         <f t="shared" si="0"/>
         <v>-18.864180483803331</v>
       </c>
-      <c r="O10" s="94"/>
-      <c r="P10" s="95"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="94"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
@@ -5956,22 +5959,22 @@
       <c r="G11" s="64">
         <v>12</v>
       </c>
-      <c r="H11" s="94">
+      <c r="H11" s="91">
         <v>2.4899310910897801</v>
       </c>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="94">
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91">
         <v>11.0540373868809</v>
       </c>
-      <c r="L11" s="94"/>
-      <c r="M11" s="94"/>
-      <c r="N11" s="94">
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91">
         <f t="shared" si="0"/>
         <v>-7.1634803480205571</v>
       </c>
-      <c r="O11" s="94"/>
-      <c r="P11" s="95"/>
+      <c r="O11" s="91"/>
+      <c r="P11" s="94"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
@@ -5989,22 +5992,22 @@
       <c r="G12" s="64">
         <v>14</v>
       </c>
-      <c r="H12" s="94">
+      <c r="H12" s="91">
         <v>2.8029840185010202</v>
       </c>
-      <c r="I12" s="94"/>
-      <c r="J12" s="94"/>
-      <c r="K12" s="94">
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91">
         <v>10.654835506500699</v>
       </c>
-      <c r="L12" s="94"/>
-      <c r="M12" s="94"/>
-      <c r="N12" s="94">
+      <c r="L12" s="91"/>
+      <c r="M12" s="91"/>
+      <c r="N12" s="91">
         <f t="shared" si="0"/>
         <v>2.4675893078542419</v>
       </c>
-      <c r="O12" s="94"/>
-      <c r="P12" s="95"/>
+      <c r="O12" s="91"/>
+      <c r="P12" s="94"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
@@ -6022,22 +6025,22 @@
       <c r="G13" s="64">
         <v>16</v>
       </c>
-      <c r="H13" s="94">
+      <c r="H13" s="91">
         <v>3.1823014852331202</v>
       </c>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94">
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91">
         <v>10.2756222546542</v>
       </c>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="94">
+      <c r="L13" s="91"/>
+      <c r="M13" s="91"/>
+      <c r="N13" s="91">
         <f t="shared" si="0"/>
         <v>7.6717047852202063</v>
       </c>
-      <c r="O13" s="94"/>
-      <c r="P13" s="95"/>
+      <c r="O13" s="91"/>
+      <c r="P13" s="94"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
@@ -6055,22 +6058,22 @@
       <c r="G14" s="64">
         <v>18</v>
       </c>
-      <c r="H14" s="94">
+      <c r="H14" s="91">
         <v>3.6522361008546498</v>
       </c>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
-      <c r="K14" s="94">
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91">
         <v>10.136937771164201</v>
       </c>
-      <c r="L14" s="94"/>
-      <c r="M14" s="94"/>
-      <c r="N14" s="94">
+      <c r="L14" s="91"/>
+      <c r="M14" s="91"/>
+      <c r="N14" s="91">
         <f t="shared" si="0"/>
         <v>10.744912968269915</v>
       </c>
-      <c r="O14" s="94"/>
-      <c r="P14" s="95"/>
+      <c r="O14" s="91"/>
+      <c r="P14" s="94"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
@@ -6088,22 +6091,22 @@
       <c r="G15" s="64">
         <v>20</v>
       </c>
-      <c r="H15" s="94">
+      <c r="H15" s="91">
         <v>4.1825961651790404</v>
       </c>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="94">
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="91">
         <v>10.278423254533401</v>
       </c>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="94">
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91">
         <f t="shared" si="0"/>
         <v>14.594385963685525</v>
       </c>
-      <c r="O15" s="94"/>
-      <c r="P15" s="95"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="94"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
@@ -6121,22 +6124,22 @@
       <c r="G16" s="64">
         <v>22</v>
       </c>
-      <c r="H16" s="94">
+      <c r="H16" s="91">
         <v>4.6954395039810901</v>
       </c>
-      <c r="I16" s="94"/>
-      <c r="J16" s="94"/>
-      <c r="K16" s="94">
+      <c r="I16" s="91"/>
+      <c r="J16" s="91"/>
+      <c r="K16" s="91">
         <v>10.1166039586804</v>
       </c>
-      <c r="L16" s="94"/>
-      <c r="M16" s="94"/>
-      <c r="N16" s="94">
+      <c r="L16" s="91"/>
+      <c r="M16" s="91"/>
+      <c r="N16" s="91">
         <f t="shared" si="0"/>
         <v>15.584193157614807</v>
       </c>
-      <c r="O16" s="94"/>
-      <c r="P16" s="95"/>
+      <c r="O16" s="91"/>
+      <c r="P16" s="94"/>
     </row>
     <row r="17" spans="1:53" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
@@ -6154,22 +6157,22 @@
       <c r="G17" s="65">
         <v>24</v>
       </c>
-      <c r="H17" s="96">
+      <c r="H17" s="95">
         <v>5.4222893772893803</v>
       </c>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96">
+      <c r="I17" s="95"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95">
         <v>10.961779173207701</v>
       </c>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96">
+      <c r="L17" s="95"/>
+      <c r="M17" s="95"/>
+      <c r="N17" s="95">
         <f t="shared" si="0"/>
         <v>14.835418392215674</v>
       </c>
-      <c r="O17" s="96"/>
-      <c r="P17" s="97"/>
+      <c r="O17" s="95"/>
+      <c r="P17" s="96"/>
     </row>
     <row r="18" spans="1:53" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -6184,60 +6187,60 @@
       <c r="B19" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85"/>
-      <c r="P19" s="85"/>
-      <c r="Q19" s="85"/>
-      <c r="R19" s="85"/>
-      <c r="S19" s="85"/>
-      <c r="T19" s="85"/>
-      <c r="U19" s="85"/>
-      <c r="V19" s="85"/>
-      <c r="W19" s="85"/>
-      <c r="X19" s="85"/>
-      <c r="Y19" s="85"/>
-      <c r="Z19" s="85"/>
-      <c r="AA19" s="86"/>
-      <c r="AC19" s="84" t="s">
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
+      <c r="G19" s="109"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="109"/>
+      <c r="K19" s="109"/>
+      <c r="L19" s="109"/>
+      <c r="M19" s="109"/>
+      <c r="N19" s="109"/>
+      <c r="O19" s="109"/>
+      <c r="P19" s="109"/>
+      <c r="Q19" s="109"/>
+      <c r="R19" s="109"/>
+      <c r="S19" s="109"/>
+      <c r="T19" s="109"/>
+      <c r="U19" s="109"/>
+      <c r="V19" s="109"/>
+      <c r="W19" s="109"/>
+      <c r="X19" s="109"/>
+      <c r="Y19" s="109"/>
+      <c r="Z19" s="109"/>
+      <c r="AA19" s="110"/>
+      <c r="AC19" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="AD19" s="85"/>
-      <c r="AE19" s="85"/>
-      <c r="AF19" s="85"/>
-      <c r="AG19" s="85"/>
-      <c r="AH19" s="85"/>
-      <c r="AI19" s="85"/>
-      <c r="AJ19" s="85"/>
-      <c r="AK19" s="85"/>
-      <c r="AL19" s="85"/>
-      <c r="AM19" s="85"/>
-      <c r="AN19" s="85"/>
-      <c r="AO19" s="85"/>
-      <c r="AP19" s="85"/>
-      <c r="AQ19" s="85"/>
-      <c r="AR19" s="85"/>
-      <c r="AS19" s="85"/>
-      <c r="AT19" s="85"/>
-      <c r="AU19" s="85"/>
-      <c r="AV19" s="85"/>
-      <c r="AW19" s="85"/>
-      <c r="AX19" s="85"/>
-      <c r="AY19" s="85"/>
-      <c r="AZ19" s="85"/>
-      <c r="BA19" s="86"/>
+      <c r="AD19" s="109"/>
+      <c r="AE19" s="109"/>
+      <c r="AF19" s="109"/>
+      <c r="AG19" s="109"/>
+      <c r="AH19" s="109"/>
+      <c r="AI19" s="109"/>
+      <c r="AJ19" s="109"/>
+      <c r="AK19" s="109"/>
+      <c r="AL19" s="109"/>
+      <c r="AM19" s="109"/>
+      <c r="AN19" s="109"/>
+      <c r="AO19" s="109"/>
+      <c r="AP19" s="109"/>
+      <c r="AQ19" s="109"/>
+      <c r="AR19" s="109"/>
+      <c r="AS19" s="109"/>
+      <c r="AT19" s="109"/>
+      <c r="AU19" s="109"/>
+      <c r="AV19" s="109"/>
+      <c r="AW19" s="109"/>
+      <c r="AX19" s="109"/>
+      <c r="AY19" s="109"/>
+      <c r="AZ19" s="109"/>
+      <c r="BA19" s="110"/>
     </row>
     <row r="20" spans="1:53" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -8182,47 +8185,47 @@
       <c r="B34" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
-      <c r="H34" s="88"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="88"/>
-      <c r="K34" s="88"/>
-      <c r="L34" s="88"/>
-      <c r="M34" s="88"/>
-      <c r="N34" s="88"/>
-      <c r="O34" s="88"/>
-      <c r="P34" s="88"/>
-      <c r="Q34" s="88"/>
-      <c r="R34" s="88"/>
-      <c r="S34" s="88"/>
-      <c r="T34" s="89"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="112"/>
+      <c r="H34" s="112"/>
+      <c r="I34" s="112"/>
+      <c r="J34" s="112"/>
+      <c r="K34" s="112"/>
+      <c r="L34" s="112"/>
+      <c r="M34" s="112"/>
+      <c r="N34" s="112"/>
+      <c r="O34" s="112"/>
+      <c r="P34" s="112"/>
+      <c r="Q34" s="112"/>
+      <c r="R34" s="112"/>
+      <c r="S34" s="112"/>
+      <c r="T34" s="113"/>
       <c r="U34" s="8"/>
-      <c r="V34" s="106" t="s">
+      <c r="V34" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="W34" s="107"/>
-      <c r="X34" s="107"/>
-      <c r="Y34" s="107"/>
-      <c r="Z34" s="107"/>
-      <c r="AA34" s="107"/>
-      <c r="AB34" s="107"/>
-      <c r="AC34" s="107"/>
-      <c r="AD34" s="107"/>
-      <c r="AE34" s="107"/>
-      <c r="AF34" s="107"/>
-      <c r="AG34" s="107"/>
-      <c r="AH34" s="107"/>
-      <c r="AI34" s="107"/>
-      <c r="AJ34" s="107"/>
-      <c r="AK34" s="107"/>
-      <c r="AL34" s="107"/>
-      <c r="AM34" s="108"/>
+      <c r="W34" s="116"/>
+      <c r="X34" s="116"/>
+      <c r="Y34" s="116"/>
+      <c r="Z34" s="116"/>
+      <c r="AA34" s="116"/>
+      <c r="AB34" s="116"/>
+      <c r="AC34" s="116"/>
+      <c r="AD34" s="116"/>
+      <c r="AE34" s="116"/>
+      <c r="AF34" s="116"/>
+      <c r="AG34" s="116"/>
+      <c r="AH34" s="116"/>
+      <c r="AI34" s="116"/>
+      <c r="AJ34" s="116"/>
+      <c r="AK34" s="116"/>
+      <c r="AL34" s="116"/>
+      <c r="AM34" s="117"/>
       <c r="AN34" s="10"/>
     </row>
     <row r="35" spans="1:40" ht="33" thickBot="1" x14ac:dyDescent="0.25">
@@ -9711,31 +9714,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N11:P11"/>
     <mergeCell ref="C19:AA19"/>
     <mergeCell ref="AC19:BA19"/>
     <mergeCell ref="V34:AM34"/>
@@ -9752,6 +9730,31 @@
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="N17:P17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9836,18 +9839,18 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="98" t="s">
+      <c r="G5" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="100"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="99"/>
     </row>
     <row r="6" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
@@ -9869,21 +9872,21 @@
       <c r="G6" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="109" t="s">
+      <c r="H6" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="101" t="s">
+      <c r="I6" s="118"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101" t="s">
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="101"/>
-      <c r="P6" s="102"/>
+      <c r="O6" s="100"/>
+      <c r="P6" s="101"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
@@ -9901,22 +9904,22 @@
       <c r="G7" s="66">
         <v>4</v>
       </c>
-      <c r="H7" s="103">
+      <c r="H7" s="102">
         <v>0.67820685919950896</v>
       </c>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="103">
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="102">
         <v>5.7430016008129297</v>
       </c>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
-      <c r="N7" s="103">
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102">
         <f>D7*180/PI()</f>
         <v>6.1225167931085114</v>
       </c>
-      <c r="O7" s="103"/>
-      <c r="P7" s="104"/>
+      <c r="O7" s="102"/>
+      <c r="P7" s="103"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
@@ -9934,22 +9937,22 @@
       <c r="G8" s="64">
         <v>6</v>
       </c>
-      <c r="H8" s="94">
+      <c r="H8" s="91">
         <v>0.84278924873573602</v>
       </c>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94">
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91">
         <v>5.7070462668519601</v>
       </c>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="94">
+      <c r="L8" s="91"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="91">
         <f t="shared" ref="N8:N17" si="0">D8*180/PI()</f>
         <v>5.0136629885353061</v>
       </c>
-      <c r="O8" s="94"/>
-      <c r="P8" s="95"/>
+      <c r="O8" s="91"/>
+      <c r="P8" s="94"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
@@ -9967,22 +9970,22 @@
       <c r="G9" s="64">
         <v>8</v>
       </c>
-      <c r="H9" s="94">
+      <c r="H9" s="91">
         <v>1.0825566519662999</v>
       </c>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94">
+      <c r="I9" s="91"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="91">
         <v>5.8584898723381196</v>
       </c>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="94">
+      <c r="L9" s="91"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="91">
         <f t="shared" si="0"/>
         <v>2.8008474964219201</v>
       </c>
-      <c r="O9" s="94"/>
-      <c r="P9" s="95"/>
+      <c r="O9" s="91"/>
+      <c r="P9" s="94"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
@@ -10000,22 +10003,22 @@
       <c r="G10" s="64">
         <v>10</v>
       </c>
-      <c r="H10" s="94">
+      <c r="H10" s="91">
         <v>1.3771476416737201</v>
       </c>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94">
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91">
         <v>6.1240859365714897</v>
       </c>
-      <c r="L10" s="94"/>
-      <c r="M10" s="94"/>
-      <c r="N10" s="94">
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91">
         <f t="shared" si="0"/>
         <v>0.54705779049602898</v>
       </c>
-      <c r="O10" s="94"/>
-      <c r="P10" s="95"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="94"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
@@ -10033,22 +10036,22 @@
       <c r="G11" s="64">
         <v>12</v>
       </c>
-      <c r="H11" s="94">
+      <c r="H11" s="91">
         <v>1.7289219331503001</v>
       </c>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="94">
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91">
         <v>6.4803219829163901</v>
       </c>
-      <c r="L11" s="94"/>
-      <c r="M11" s="94"/>
-      <c r="N11" s="94">
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91">
         <f t="shared" si="0"/>
         <v>-0.91911848771942295</v>
       </c>
-      <c r="O11" s="94"/>
-      <c r="P11" s="95"/>
+      <c r="O11" s="91"/>
+      <c r="P11" s="94"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
@@ -10066,22 +10069,22 @@
       <c r="G12" s="64">
         <v>14</v>
       </c>
-      <c r="H12" s="94">
+      <c r="H12" s="91">
         <v>2.1097219363978699</v>
       </c>
-      <c r="I12" s="94"/>
-      <c r="J12" s="94"/>
-      <c r="K12" s="94">
+      <c r="I12" s="91"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91">
         <v>6.8496118637543404</v>
       </c>
-      <c r="L12" s="94"/>
-      <c r="M12" s="94"/>
-      <c r="N12" s="94">
+      <c r="L12" s="91"/>
+      <c r="M12" s="91"/>
+      <c r="N12" s="91">
         <f t="shared" si="0"/>
         <v>-0.99801098875008087</v>
       </c>
-      <c r="O12" s="94"/>
-      <c r="P12" s="95"/>
+      <c r="O12" s="91"/>
+      <c r="P12" s="94"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
@@ -10099,22 +10102,22 @@
       <c r="G13" s="64">
         <v>16</v>
       </c>
-      <c r="H13" s="94">
+      <c r="H13" s="91">
         <v>2.5091502791257301</v>
       </c>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94">
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91">
         <v>7.1951041189657099</v>
       </c>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="94">
+      <c r="L13" s="91"/>
+      <c r="M13" s="91"/>
+      <c r="N13" s="91">
         <f t="shared" si="0"/>
         <v>-0.20205712088628408</v>
       </c>
-      <c r="O13" s="94"/>
-      <c r="P13" s="95"/>
+      <c r="O13" s="91"/>
+      <c r="P13" s="94"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
@@ -10132,22 +10135,22 @@
       <c r="G14" s="64">
         <v>18</v>
       </c>
-      <c r="H14" s="94">
+      <c r="H14" s="91">
         <v>2.9963842683238702</v>
       </c>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
-      <c r="K14" s="94">
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91">
         <v>7.6467174212998801</v>
       </c>
-      <c r="L14" s="94"/>
-      <c r="M14" s="94"/>
-      <c r="N14" s="94">
+      <c r="L14" s="91"/>
+      <c r="M14" s="91"/>
+      <c r="N14" s="91">
         <f t="shared" si="0"/>
         <v>2.1339105565932037</v>
       </c>
-      <c r="O14" s="94"/>
-      <c r="P14" s="95"/>
+      <c r="O14" s="91"/>
+      <c r="P14" s="94"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
@@ -10165,22 +10168,22 @@
       <c r="G15" s="64">
         <v>20</v>
       </c>
-      <c r="H15" s="94">
+      <c r="H15" s="91">
         <v>3.5305936369636099</v>
       </c>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="94">
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="91">
         <v>8.2009401919392602</v>
       </c>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="94">
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91">
         <f t="shared" si="0"/>
         <v>6.8764793451458139</v>
       </c>
-      <c r="O15" s="94"/>
-      <c r="P15" s="95"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="94"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
@@ -10198,22 +10201,22 @@
       <c r="G16" s="64">
         <v>22</v>
       </c>
-      <c r="H16" s="94">
+      <c r="H16" s="91">
         <v>4.0745393772151202</v>
       </c>
-      <c r="I16" s="94"/>
-      <c r="J16" s="94"/>
-      <c r="K16" s="94">
+      <c r="I16" s="91"/>
+      <c r="J16" s="91"/>
+      <c r="K16" s="91">
         <v>8.7446999567920294</v>
       </c>
-      <c r="L16" s="94"/>
-      <c r="M16" s="94"/>
-      <c r="N16" s="94">
+      <c r="L16" s="91"/>
+      <c r="M16" s="91"/>
+      <c r="N16" s="91">
         <f t="shared" si="0"/>
         <v>15.480834806481251</v>
       </c>
-      <c r="O16" s="94"/>
-      <c r="P16" s="95"/>
+      <c r="O16" s="91"/>
+      <c r="P16" s="94"/>
     </row>
     <row r="17" spans="1:56" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
@@ -10231,22 +10234,22 @@
       <c r="G17" s="65">
         <v>24</v>
       </c>
-      <c r="H17" s="96">
+      <c r="H17" s="95">
         <v>4.3369975980750901</v>
       </c>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96">
+      <c r="I17" s="95"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95">
         <v>9.0083702498509695</v>
       </c>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96">
+      <c r="L17" s="95"/>
+      <c r="M17" s="95"/>
+      <c r="N17" s="95">
         <f t="shared" si="0"/>
         <v>21.897414333852847</v>
       </c>
-      <c r="O17" s="96"/>
-      <c r="P17" s="97"/>
+      <c r="O17" s="95"/>
+      <c r="P17" s="96"/>
     </row>
     <row r="18" spans="1:56" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -10261,60 +10264,60 @@
       <c r="B19" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85"/>
-      <c r="P19" s="85"/>
-      <c r="Q19" s="85"/>
-      <c r="R19" s="85"/>
-      <c r="S19" s="85"/>
-      <c r="T19" s="85"/>
-      <c r="U19" s="85"/>
-      <c r="V19" s="85"/>
-      <c r="W19" s="85"/>
-      <c r="X19" s="85"/>
-      <c r="Y19" s="85"/>
-      <c r="Z19" s="85"/>
-      <c r="AA19" s="86"/>
-      <c r="AF19" s="84" t="s">
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
+      <c r="G19" s="109"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="109"/>
+      <c r="K19" s="109"/>
+      <c r="L19" s="109"/>
+      <c r="M19" s="109"/>
+      <c r="N19" s="109"/>
+      <c r="O19" s="109"/>
+      <c r="P19" s="109"/>
+      <c r="Q19" s="109"/>
+      <c r="R19" s="109"/>
+      <c r="S19" s="109"/>
+      <c r="T19" s="109"/>
+      <c r="U19" s="109"/>
+      <c r="V19" s="109"/>
+      <c r="W19" s="109"/>
+      <c r="X19" s="109"/>
+      <c r="Y19" s="109"/>
+      <c r="Z19" s="109"/>
+      <c r="AA19" s="110"/>
+      <c r="AF19" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="AG19" s="85"/>
-      <c r="AH19" s="85"/>
-      <c r="AI19" s="85"/>
-      <c r="AJ19" s="85"/>
-      <c r="AK19" s="85"/>
-      <c r="AL19" s="85"/>
-      <c r="AM19" s="85"/>
-      <c r="AN19" s="85"/>
-      <c r="AO19" s="85"/>
-      <c r="AP19" s="85"/>
-      <c r="AQ19" s="85"/>
-      <c r="AR19" s="85"/>
-      <c r="AS19" s="85"/>
-      <c r="AT19" s="85"/>
-      <c r="AU19" s="85"/>
-      <c r="AV19" s="85"/>
-      <c r="AW19" s="85"/>
-      <c r="AX19" s="85"/>
-      <c r="AY19" s="85"/>
-      <c r="AZ19" s="85"/>
-      <c r="BA19" s="85"/>
-      <c r="BB19" s="85"/>
-      <c r="BC19" s="85"/>
-      <c r="BD19" s="86"/>
+      <c r="AG19" s="109"/>
+      <c r="AH19" s="109"/>
+      <c r="AI19" s="109"/>
+      <c r="AJ19" s="109"/>
+      <c r="AK19" s="109"/>
+      <c r="AL19" s="109"/>
+      <c r="AM19" s="109"/>
+      <c r="AN19" s="109"/>
+      <c r="AO19" s="109"/>
+      <c r="AP19" s="109"/>
+      <c r="AQ19" s="109"/>
+      <c r="AR19" s="109"/>
+      <c r="AS19" s="109"/>
+      <c r="AT19" s="109"/>
+      <c r="AU19" s="109"/>
+      <c r="AV19" s="109"/>
+      <c r="AW19" s="109"/>
+      <c r="AX19" s="109"/>
+      <c r="AY19" s="109"/>
+      <c r="AZ19" s="109"/>
+      <c r="BA19" s="109"/>
+      <c r="BB19" s="109"/>
+      <c r="BC19" s="109"/>
+      <c r="BD19" s="110"/>
     </row>
     <row r="20" spans="1:56" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -12218,43 +12221,43 @@
       <c r="B34" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="84" t="s">
+      <c r="C34" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="85"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="85"/>
-      <c r="I34" s="85"/>
-      <c r="J34" s="85"/>
-      <c r="K34" s="85"/>
-      <c r="L34" s="85"/>
-      <c r="M34" s="85"/>
-      <c r="N34" s="85"/>
-      <c r="O34" s="85"/>
-      <c r="P34" s="85"/>
-      <c r="Q34" s="85"/>
-      <c r="R34" s="86"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="109"/>
+      <c r="K34" s="109"/>
+      <c r="L34" s="109"/>
+      <c r="M34" s="109"/>
+      <c r="N34" s="109"/>
+      <c r="O34" s="109"/>
+      <c r="P34" s="109"/>
+      <c r="Q34" s="109"/>
+      <c r="R34" s="110"/>
       <c r="S34" s="20"/>
-      <c r="T34" s="84" t="s">
+      <c r="T34" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="U34" s="85"/>
-      <c r="V34" s="85"/>
-      <c r="W34" s="85"/>
-      <c r="X34" s="85"/>
-      <c r="Y34" s="85"/>
-      <c r="Z34" s="85"/>
-      <c r="AA34" s="85"/>
-      <c r="AB34" s="85"/>
-      <c r="AC34" s="85"/>
-      <c r="AD34" s="85"/>
-      <c r="AE34" s="85"/>
-      <c r="AF34" s="85"/>
-      <c r="AG34" s="85"/>
-      <c r="AH34" s="85"/>
-      <c r="AI34" s="86"/>
+      <c r="U34" s="109"/>
+      <c r="V34" s="109"/>
+      <c r="W34" s="109"/>
+      <c r="X34" s="109"/>
+      <c r="Y34" s="109"/>
+      <c r="Z34" s="109"/>
+      <c r="AA34" s="109"/>
+      <c r="AB34" s="109"/>
+      <c r="AC34" s="109"/>
+      <c r="AD34" s="109"/>
+      <c r="AE34" s="109"/>
+      <c r="AF34" s="109"/>
+      <c r="AG34" s="109"/>
+      <c r="AH34" s="109"/>
+      <c r="AI34" s="110"/>
     </row>
     <row r="35" spans="1:35" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
@@ -13498,31 +13501,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N11:P11"/>
     <mergeCell ref="C19:AA19"/>
     <mergeCell ref="AF19:BD19"/>
     <mergeCell ref="C34:R34"/>
@@ -13539,6 +13517,31 @@
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="N17:P17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>